<commit_message>
Updated Last Week's Hours
Standard hour count.
</commit_message>
<xml_diff>
--- a/CS297-TimeTracking.xlsx
+++ b/CS297-TimeTracking.xlsx
@@ -171,7 +171,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -229,25 +229,25 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">B4</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">D4</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">F4</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I4" s="0" t="n">
         <f aca="false">H4</f>
@@ -260,11 +260,11 @@
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">B5+C4</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">D5+E4</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">F5</f>
@@ -281,11 +281,11 @@
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">B6+C5</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">D6+E5</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">F6</f>
@@ -302,11 +302,11 @@
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">B7+C6</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7+E6</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">F7</f>
@@ -323,11 +323,11 @@
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">B8+C7</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">F8</f>
@@ -344,11 +344,11 @@
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9+C8</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">F9</f>
@@ -365,11 +365,11 @@
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10+C9</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">F10</f>
@@ -386,11 +386,11 @@
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">B11+C10</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">F11</f>
@@ -407,11 +407,11 @@
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">B12+C11</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">F12</f>
@@ -428,11 +428,11 @@
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">B13+C12</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">F13</f>

</xml_diff>